<commit_message>
Add, Update, Delete category and product feature
</commit_message>
<xml_diff>
--- a/Management_Book/BookData.xlsx
+++ b/Management_Book/BookData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minht\Desktop\GitHub\book-store-management\Management_Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7DB6BFD-C457-4075-B8DF-B949B7C6DC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B77577-E0F6-4175-B0EC-A5351C428601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8445" yWindow="7050" windowWidth="28800" windowHeight="15435" xr2:uid="{C18C0562-95FB-4E33-A1A3-47AE3216B614}"/>
+    <workbookView xWindow="1440" yWindow="8445" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{C18C0562-95FB-4E33-A1A3-47AE3216B614}"/>
   </bookViews>
   <sheets>
     <sheet name="Category" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="75">
   <si>
     <t>Nhà Giả Kim</t>
   </si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>Thiếu nhi</t>
+  </si>
+  <si>
+    <t>Cost</t>
   </si>
 </sst>
 </file>
@@ -641,7 +644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C076A39E-B6EA-426D-8D59-67DB3CACB31C}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -697,20 +700,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A293813D-AF92-4680-A3F8-6CFD7E6CAA96}">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>64</v>
       </c>
@@ -724,13 +727,16 @@
         <v>67</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -744,11 +750,15 @@
         <v>59000</v>
       </c>
       <c r="E2" s="2">
+        <f>D2 - (D2 * 20 / 100)</f>
+        <v>47200</v>
+      </c>
+      <c r="F2" s="2">
         <v>39</v>
       </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -762,11 +772,15 @@
         <v>147000</v>
       </c>
       <c r="E3" s="2">
+        <f t="shared" ref="E3:E65" si="0">D3 - (D3 * 20 / 100)</f>
+        <v>117600</v>
+      </c>
+      <c r="F3" s="2">
         <v>41</v>
       </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -780,11 +794,15 @@
         <v>130000</v>
       </c>
       <c r="E4" s="2">
+        <f t="shared" si="0"/>
+        <v>104000</v>
+      </c>
+      <c r="F4" s="2">
         <v>43</v>
       </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -798,11 +816,15 @@
         <v>63900</v>
       </c>
       <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>51120</v>
+      </c>
+      <c r="F5" s="2">
         <v>45</v>
       </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -816,11 +838,15 @@
         <v>957000</v>
       </c>
       <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>765600</v>
+      </c>
+      <c r="F6" s="2">
         <v>47</v>
       </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -834,11 +860,15 @@
         <v>68000</v>
       </c>
       <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>54400</v>
+      </c>
+      <c r="F7" s="2">
         <v>49</v>
       </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -852,11 +882,15 @@
         <v>63000</v>
       </c>
       <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>50400</v>
+      </c>
+      <c r="F8" s="2">
         <v>51</v>
       </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -870,11 +904,15 @@
         <v>92000</v>
       </c>
       <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>73600</v>
+      </c>
+      <c r="F9" s="2">
         <v>53</v>
       </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -888,11 +926,15 @@
         <v>64700</v>
       </c>
       <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>51760</v>
+      </c>
+      <c r="F10" s="2">
         <v>55</v>
       </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -906,11 +948,15 @@
         <v>331500</v>
       </c>
       <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>265200</v>
+      </c>
+      <c r="F11" s="2">
         <v>57</v>
       </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -924,11 +970,15 @@
         <v>81000</v>
       </c>
       <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>64800</v>
+      </c>
+      <c r="F12" s="2">
         <v>59</v>
       </c>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -942,11 +992,15 @@
         <v>93000</v>
       </c>
       <c r="E13" s="2">
+        <f t="shared" si="0"/>
+        <v>74400</v>
+      </c>
+      <c r="F13" s="2">
         <v>61</v>
       </c>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -960,11 +1014,15 @@
         <v>76800</v>
       </c>
       <c r="E14" s="2">
+        <f t="shared" si="0"/>
+        <v>61440</v>
+      </c>
+      <c r="F14" s="2">
         <v>63</v>
       </c>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -978,11 +1036,15 @@
         <v>67000</v>
       </c>
       <c r="E15" s="2">
+        <f t="shared" si="0"/>
+        <v>53600</v>
+      </c>
+      <c r="F15" s="2">
         <v>65</v>
       </c>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -996,11 +1058,15 @@
         <v>77000</v>
       </c>
       <c r="E16" s="2">
+        <f t="shared" si="0"/>
+        <v>61600</v>
+      </c>
+      <c r="F16" s="2">
         <v>67</v>
       </c>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1014,11 +1080,15 @@
         <v>74100</v>
       </c>
       <c r="E17" s="2">
+        <f t="shared" si="0"/>
+        <v>59280</v>
+      </c>
+      <c r="F17" s="2">
         <v>69</v>
       </c>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1032,11 +1102,15 @@
         <v>100000</v>
       </c>
       <c r="E18" s="2">
-        <v>71</v>
-      </c>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>80000</v>
+      </c>
+      <c r="F18" s="2">
+        <v>71</v>
+      </c>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1050,11 +1124,15 @@
         <v>33400</v>
       </c>
       <c r="E19" s="2">
+        <f t="shared" si="0"/>
+        <v>26720</v>
+      </c>
+      <c r="F19" s="2">
         <v>73</v>
       </c>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1068,11 +1146,15 @@
         <v>76000</v>
       </c>
       <c r="E20" s="2">
+        <f t="shared" si="0"/>
+        <v>60800</v>
+      </c>
+      <c r="F20" s="2">
         <v>75</v>
       </c>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1086,11 +1168,15 @@
         <v>45000</v>
       </c>
       <c r="E21" s="2">
+        <f t="shared" si="0"/>
+        <v>36000</v>
+      </c>
+      <c r="F21" s="2">
         <v>77</v>
       </c>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1104,11 +1190,15 @@
         <v>49000</v>
       </c>
       <c r="E22" s="2">
+        <f t="shared" si="0"/>
+        <v>39200</v>
+      </c>
+      <c r="F22" s="2">
         <v>79</v>
       </c>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1122,11 +1212,15 @@
         <v>96000</v>
       </c>
       <c r="E23" s="2">
+        <f t="shared" si="0"/>
+        <v>76800</v>
+      </c>
+      <c r="F23" s="2">
         <v>81</v>
       </c>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1140,11 +1234,15 @@
         <v>113000</v>
       </c>
       <c r="E24" s="2">
+        <f t="shared" si="0"/>
+        <v>90400</v>
+      </c>
+      <c r="F24" s="2">
         <v>83</v>
       </c>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1158,11 +1256,15 @@
         <v>70000</v>
       </c>
       <c r="E25" s="2">
+        <f t="shared" si="0"/>
+        <v>56000</v>
+      </c>
+      <c r="F25" s="2">
         <v>85</v>
       </c>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1176,11 +1278,15 @@
         <v>70000</v>
       </c>
       <c r="E26" s="2">
+        <f t="shared" si="0"/>
+        <v>56000</v>
+      </c>
+      <c r="F26" s="2">
         <v>87</v>
       </c>
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1194,11 +1300,15 @@
         <v>205000</v>
       </c>
       <c r="E27" s="2">
+        <f t="shared" si="0"/>
+        <v>164000</v>
+      </c>
+      <c r="F27" s="2">
         <v>84</v>
       </c>
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1212,11 +1322,15 @@
         <v>88000</v>
       </c>
       <c r="E28" s="2">
+        <f t="shared" si="0"/>
+        <v>70400</v>
+      </c>
+      <c r="F28" s="2">
         <v>81</v>
       </c>
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1230,11 +1344,15 @@
         <v>205000</v>
       </c>
       <c r="E29" s="2">
+        <f t="shared" si="0"/>
+        <v>164000</v>
+      </c>
+      <c r="F29" s="2">
         <v>78</v>
       </c>
-      <c r="F29" s="2"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1248,11 +1366,15 @@
         <v>298000</v>
       </c>
       <c r="E30" s="2">
+        <f t="shared" si="0"/>
+        <v>238400</v>
+      </c>
+      <c r="F30" s="2">
         <v>75</v>
       </c>
-      <c r="F30" s="2"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1266,11 +1388,15 @@
         <v>299000</v>
       </c>
       <c r="E31" s="2">
+        <f t="shared" si="0"/>
+        <v>239200</v>
+      </c>
+      <c r="F31" s="2">
         <v>72</v>
       </c>
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1284,11 +1410,15 @@
         <v>299000</v>
       </c>
       <c r="E32" s="2">
+        <f t="shared" si="0"/>
+        <v>239200</v>
+      </c>
+      <c r="F32" s="2">
         <v>69</v>
       </c>
-      <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1302,11 +1432,15 @@
         <v>233000</v>
       </c>
       <c r="E33" s="2">
+        <f t="shared" si="0"/>
+        <v>186400</v>
+      </c>
+      <c r="F33" s="2">
         <v>66</v>
       </c>
-      <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1320,11 +1454,15 @@
         <v>599000</v>
       </c>
       <c r="E34" s="2">
+        <f t="shared" si="0"/>
+        <v>479200</v>
+      </c>
+      <c r="F34" s="2">
         <v>63</v>
       </c>
-      <c r="F34" s="2"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1338,11 +1476,15 @@
         <v>149000</v>
       </c>
       <c r="E35" s="2">
+        <f t="shared" si="0"/>
+        <v>119200</v>
+      </c>
+      <c r="F35" s="2">
         <v>60</v>
       </c>
-      <c r="F35" s="2"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1356,11 +1498,15 @@
         <v>323000</v>
       </c>
       <c r="E36" s="2">
+        <f t="shared" si="0"/>
+        <v>258400</v>
+      </c>
+      <c r="F36" s="2">
         <v>57</v>
       </c>
-      <c r="F36" s="2"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1374,11 +1520,15 @@
         <v>96000</v>
       </c>
       <c r="E37" s="2">
+        <f t="shared" si="0"/>
+        <v>76800</v>
+      </c>
+      <c r="F37" s="2">
         <v>54</v>
       </c>
-      <c r="F37" s="2"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -1392,11 +1542,15 @@
         <v>45000</v>
       </c>
       <c r="E38" s="2">
+        <f t="shared" si="0"/>
+        <v>36000</v>
+      </c>
+      <c r="F38" s="2">
         <v>51</v>
       </c>
-      <c r="F38" s="2"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -1410,11 +1564,15 @@
         <v>104000</v>
       </c>
       <c r="E39" s="2">
+        <f t="shared" si="0"/>
+        <v>83200</v>
+      </c>
+      <c r="F39" s="2">
         <v>48</v>
       </c>
-      <c r="F39" s="2"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39" s="2"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -1428,11 +1586,15 @@
         <v>83000</v>
       </c>
       <c r="E40" s="2">
+        <f t="shared" si="0"/>
+        <v>66400</v>
+      </c>
+      <c r="F40" s="2">
         <v>45</v>
       </c>
-      <c r="F40" s="2"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -1446,11 +1608,15 @@
         <v>86000</v>
       </c>
       <c r="E41" s="2">
+        <f t="shared" si="0"/>
+        <v>68800</v>
+      </c>
+      <c r="F41" s="2">
         <v>42</v>
       </c>
-      <c r="F41" s="2"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -1464,11 +1630,15 @@
         <v>155000</v>
       </c>
       <c r="E42" s="2">
+        <f t="shared" si="0"/>
+        <v>124000</v>
+      </c>
+      <c r="F42" s="2">
         <v>39</v>
       </c>
-      <c r="F42" s="2"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -1482,11 +1652,15 @@
         <v>131000</v>
       </c>
       <c r="E43" s="2">
+        <f t="shared" si="0"/>
+        <v>104800</v>
+      </c>
+      <c r="F43" s="2">
         <v>36</v>
       </c>
-      <c r="F43" s="2"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43" s="2"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -1500,11 +1674,15 @@
         <v>95000</v>
       </c>
       <c r="E44" s="2">
+        <f t="shared" si="0"/>
+        <v>76000</v>
+      </c>
+      <c r="F44" s="2">
         <v>33</v>
       </c>
-      <c r="F44" s="2"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44" s="2"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -1518,11 +1696,15 @@
         <v>163000</v>
       </c>
       <c r="E45" s="2">
+        <f t="shared" si="0"/>
+        <v>130400</v>
+      </c>
+      <c r="F45" s="2">
         <v>30</v>
       </c>
-      <c r="F45" s="2"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -1536,11 +1718,15 @@
         <v>60000</v>
       </c>
       <c r="E46" s="2">
+        <f t="shared" si="0"/>
+        <v>48000</v>
+      </c>
+      <c r="F46" s="2">
         <v>27</v>
       </c>
-      <c r="F46" s="2"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46" s="2"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -1554,11 +1740,15 @@
         <v>238000</v>
       </c>
       <c r="E47" s="2">
+        <f t="shared" si="0"/>
+        <v>190400</v>
+      </c>
+      <c r="F47" s="2">
         <v>24</v>
       </c>
-      <c r="F47" s="2"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47" s="2"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -1572,11 +1762,15 @@
         <v>223000</v>
       </c>
       <c r="E48" s="2">
+        <f t="shared" si="0"/>
+        <v>178400</v>
+      </c>
+      <c r="F48" s="2">
         <v>28</v>
       </c>
-      <c r="F48" s="2"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48" s="2"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -1590,11 +1784,15 @@
         <v>118000</v>
       </c>
       <c r="E49" s="2">
+        <f t="shared" si="0"/>
+        <v>94400</v>
+      </c>
+      <c r="F49" s="2">
         <v>32</v>
       </c>
-      <c r="F49" s="2"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49" s="2"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -1608,11 +1806,15 @@
         <v>60000</v>
       </c>
       <c r="E50" s="2">
+        <f t="shared" si="0"/>
+        <v>48000</v>
+      </c>
+      <c r="F50" s="2">
         <v>36</v>
       </c>
-      <c r="F50" s="2"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50" s="2"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -1626,11 +1828,15 @@
         <v>69000</v>
       </c>
       <c r="E51" s="2">
+        <f t="shared" si="0"/>
+        <v>55200</v>
+      </c>
+      <c r="F51" s="2">
         <v>40</v>
       </c>
-      <c r="F51" s="2"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51" s="2"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -1644,11 +1850,15 @@
         <v>125000</v>
       </c>
       <c r="E52" s="2">
+        <f t="shared" si="0"/>
+        <v>100000</v>
+      </c>
+      <c r="F52" s="2">
         <v>44</v>
       </c>
-      <c r="F52" s="2"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G52" s="2"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -1662,11 +1872,15 @@
         <v>59000</v>
       </c>
       <c r="E53" s="2">
+        <f t="shared" si="0"/>
+        <v>47200</v>
+      </c>
+      <c r="F53" s="2">
         <v>48</v>
       </c>
-      <c r="F53" s="2"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G53" s="2"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -1680,11 +1894,15 @@
         <v>68000</v>
       </c>
       <c r="E54" s="2">
+        <f t="shared" si="0"/>
+        <v>54400</v>
+      </c>
+      <c r="F54" s="2">
         <v>52</v>
       </c>
-      <c r="F54" s="2"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G54" s="2"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -1698,11 +1916,15 @@
         <v>63000</v>
       </c>
       <c r="E55" s="2">
+        <f t="shared" si="0"/>
+        <v>50400</v>
+      </c>
+      <c r="F55" s="2">
         <v>56</v>
       </c>
-      <c r="F55" s="2"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G55" s="2"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -1716,11 +1938,15 @@
         <v>78000</v>
       </c>
       <c r="E56" s="2">
+        <f t="shared" si="0"/>
+        <v>62400</v>
+      </c>
+      <c r="F56" s="2">
         <v>60</v>
       </c>
-      <c r="F56" s="2"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G56" s="2"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -1734,11 +1960,15 @@
         <v>63000</v>
       </c>
       <c r="E57" s="2">
+        <f t="shared" si="0"/>
+        <v>50400</v>
+      </c>
+      <c r="F57" s="2">
         <v>64</v>
       </c>
-      <c r="F57" s="2"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G57" s="2"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -1752,11 +1982,15 @@
         <v>66000</v>
       </c>
       <c r="E58" s="2">
+        <f t="shared" si="0"/>
+        <v>52800</v>
+      </c>
+      <c r="F58" s="2">
         <v>68</v>
       </c>
-      <c r="F58" s="2"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G58" s="2"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -1770,11 +2004,15 @@
         <v>63000</v>
       </c>
       <c r="E59" s="2">
+        <f t="shared" si="0"/>
+        <v>50400</v>
+      </c>
+      <c r="F59" s="2">
         <v>72</v>
       </c>
-      <c r="F59" s="2"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G59" s="2"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -1788,11 +2026,15 @@
         <v>4000</v>
       </c>
       <c r="E60" s="2">
+        <f t="shared" si="0"/>
+        <v>3200</v>
+      </c>
+      <c r="F60" s="2">
         <v>76</v>
       </c>
-      <c r="F60" s="2"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G60" s="2"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -1806,11 +2048,15 @@
         <v>44000</v>
       </c>
       <c r="E61" s="2">
+        <f t="shared" si="0"/>
+        <v>35200</v>
+      </c>
+      <c r="F61" s="2">
         <v>80</v>
       </c>
-      <c r="F61" s="2"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G61" s="2"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -1824,11 +2070,15 @@
         <v>22700</v>
       </c>
       <c r="E62" s="2">
+        <f t="shared" si="0"/>
+        <v>18160</v>
+      </c>
+      <c r="F62" s="2">
         <v>84</v>
       </c>
-      <c r="F62" s="2"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G62" s="2"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -1842,11 +2092,15 @@
         <v>41000</v>
       </c>
       <c r="E63" s="2">
+        <f t="shared" si="0"/>
+        <v>32800</v>
+      </c>
+      <c r="F63" s="2">
         <v>88</v>
       </c>
-      <c r="F63" s="2"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G63" s="2"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -1860,11 +2114,15 @@
         <v>200000</v>
       </c>
       <c r="E64" s="2">
+        <f t="shared" si="0"/>
+        <v>160000</v>
+      </c>
+      <c r="F64" s="2">
         <v>92</v>
       </c>
-      <c r="F64" s="2"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G64" s="2"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -1878,9 +2136,13 @@
         <v>44000</v>
       </c>
       <c r="E65" s="2">
+        <f t="shared" si="0"/>
+        <v>35200</v>
+      </c>
+      <c r="F65" s="2">
         <v>96</v>
       </c>
-      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>